<commit_message>
Updating the Excel Workbook
</commit_message>
<xml_diff>
--- a/ClimateHistory/USHCN Combined Raw and Modified Data.xlsx
+++ b/ClimateHistory/USHCN Combined Raw and Modified Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4dc8152b23c86b3/Climate History/2024.06.07_ClimateMonthly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{4FA342C7-3F01-4F17-8348-AF203B1C7A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54894D24-EFB7-4E0F-A834-113FF5545E3F}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{D1000FBC-87CB-482D-BB97-5B5B1F312AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6441E402-12CC-47F8-BEEE-3C3C66FC3128}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{62A43EBB-79E8-49B2-9FF1-C7E809F0319F}"/>
   </bookViews>
@@ -727,7 +727,7 @@
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -872,7 +872,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:prstDash val="sysDash"/>
               </a:ln>
@@ -1795,6 +1795,7 @@
         <c:axId val="587698168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="14"/>
           <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1902,42 +1903,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx2">
@@ -2009,7 +1980,45 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>USHCN Delta Percent of Days Over 90 Degrees Fahrenheit Between Modified and Raw Data</a:t>
+              <a:t>USHCN Percent of Days Over 90 Degrees Fahrenheit Delta Between </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Modified</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> (FLs.52j) and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Raw</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Data</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -2025,7 +2034,64 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>(Modified - Raw)</a:t>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>&gt;90 Delta </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>= </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>FLs.52j </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>- </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Raw</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2082,7 +2148,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2183,9 +2249,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="7030A0"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -3331,14 +3397,14 @@
             <a:r>
               <a:rPr lang="en-US">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>USHCN Raw Data</a:t>
+              <a:t>USHCN Raw Data </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t> Percent of Days Greater Than 90 DegF</a:t>
+              <a:t>Percent of Days Greater Than 90 DegF</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3392,7 +3458,7 @@
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4460,6 +4526,7 @@
         <c:axId val="587698168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="14"/>
           <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4567,42 +4634,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx2">
@@ -4668,7 +4705,7 @@
             <a:r>
               <a:rPr lang="en-US" b="1">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>USHCN Raw Data </a:t>
@@ -4732,7 +4769,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4804,14 +4841,13 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4865,7 +4901,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -5911,45 +5947,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -6086,7 +6089,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -6158,14 +6161,13 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -6217,9 +6219,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -7149,6 +7151,7 @@
         <c:axId val="286827624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="93"/>
           <c:min val="84"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -7272,45 +7275,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -7390,7 +7360,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>USHCN Raw Data </a:t>
@@ -7423,16 +7393,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -7505,7 +7472,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -7607,14 +7574,13 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -7668,7 +7634,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -8721,45 +8687,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -8872,16 +8805,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -8962,7 +8892,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9064,14 +8994,13 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9123,9 +9052,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -10171,45 +10100,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -10289,7 +10185,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>USHCN Raw Data </a:t>
@@ -10322,16 +10218,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -10404,7 +10297,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -10491,14 +10384,13 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10552,7 +10444,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -11605,45 +11497,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -11780,7 +11639,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -11867,14 +11726,13 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -11926,9 +11784,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -12974,45 +12832,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -13089,7 +12914,58 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Delta Maximum Temperatures Between Modified and Raw Data</a:t>
+              <a:t>Maximum Temperatures </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Delta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> Between </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Modified</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(FLs.52j) </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Raw</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> Data</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -13098,7 +12974,43 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>(Modified - Raw)</a:t>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Maximum Delta </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>= </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>FLs.52j</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Raw</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -13165,7 +13077,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -13266,9 +13178,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="7030A0"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -19856,9 +19768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19891,10 +19803,10 @@
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19922,15 +19834,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
+      <xdr:colOff>552449</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19958,15 +19870,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19994,15 +19906,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20038,7 +19950,7 @@
       <xdr:col>33</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20072,9 +19984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20102,15 +20014,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>9523</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20138,15 +20050,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4761</xdr:colOff>
+      <xdr:colOff>4760</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>4760</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20180,9 +20092,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20533,9 +20445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE716131-8715-4172-8F4A-841C230B3C0F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -20548,8 +20458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CF175E-AA12-43C7-8A6F-BAA30B18B859}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I1" activeCellId="1" sqref="A1:A130 I1:I130"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27453,8 +27363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258117E4-0E45-4FC2-9C9A-1EA2607B33EB}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" activeCellId="1" sqref="A1:A130 I1:I130"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="K1" activeCellId="1" sqref="H1:J1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34358,9 +34268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADB7F7E-6F6E-44F1-9A55-FBCA524FCF16}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>